<commit_message>
Update Cliente Solar Análise.xlsx
</commit_message>
<xml_diff>
--- a/Cliente Solar Análise.xlsx
+++ b/Cliente Solar Análise.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fc015c659b534d1/Workplace/Portfólio Análise de dados/Excel-Analise_de_expansao_solar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{3A67DC9C-4C51-466A-AA1B-27A9AAD673B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E743363-877C-48B6-8D19-4377F563D8B9}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{3A67DC9C-4C51-466A-AA1B-27A9AAD673B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB3B184-050A-4C67-B57C-4654134CF5CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{E283EC9B-F660-469F-A706-101104E76017}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{E283EC9B-F660-469F-A706-101104E76017}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo_Monitoramento" sheetId="10" r:id="rId1"/>
     <sheet name="Análise" sheetId="13" r:id="rId2"/>
-    <sheet name="dados" sheetId="12" r:id="rId3"/>
+    <sheet name="dados" sheetId="12" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="B_Vermelha">dados!$B$3</definedName>
@@ -5731,7 +5731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB52DBFC-5240-40D6-AACD-CCEDA1E6D71D}">
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
@@ -10222,7 +10222,7 @@
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>

</xml_diff>